<commit_message>
data majj + liste etape
</commit_message>
<xml_diff>
--- a/static/data/data.xlsx
+++ b/static/data/data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\GitHub\thomasmrt.github.io\static\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\safco103866\Desktop\Tools\site\thomasmrt.github.io\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BD8342-8B19-4D63-A49B-8A0974E51C0D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -18,12 +17,12 @@
     <sheet name="Queyras" sheetId="3" r:id="rId3"/>
     <sheet name="Taillefer" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="345">
   <si>
     <t>section_start</t>
   </si>
@@ -343,9 +342,6 @@
     <t>Au revoir îles Lofoten</t>
   </si>
   <si>
-    <t>Post Rando</t>
-  </si>
-  <si>
     <t>Oslo</t>
   </si>
   <si>
@@ -1046,12 +1042,27 @@
   </si>
   <si>
     <t>https://lh3.googleusercontent.com/503kqX_NRmn5kC5IKD8XS9wbdKd3d9VsBlZQlHI3r-rKU_jyLtfQSJM3kp5gL1JmcgVzY3pODFMLTq3l01d15TnErJcMMpyy6OSLZirfJBue458_0AWWUsx4LilL8lCusGU3ADgby-pgvT4nlWyNytyCzb3BOg9XEKwOlaCigYEMYbuTgijuATC44FQrGP9VK5N4AbCiii6uYd7X2-AIQ4wr6Jvi5uBn1QFE-zZFTiG9AnN0PMNIPVmoUMmgvqU-4jYg4bZNodIsrVT8bYGGRZxqT25q7f_A3LXgLMTsqv2b4D2QlCKcL90ZGHVDm4YUkUKLqGGBI_TrhBhJtktlLMJ5vPsQYZv27YaQhJAexeFatisp9QjCpffTV6aLpGdK6pszQwEfO2QwFwcOx3_XM2KclmYAKA9jp0SuyF1q43B1HFD4xe8W6TEiq8VGEw9QQfSSDAbBB93iA04lc969584Qa76PYRgi8XTBV4gSnw8jCqIGzLcmiBOBGFy94v3g7NE98VTziQqLEtuXELCbySh4fzqLxN_HHZIF18iimpTes38o_zh7jtFQl5NtLEQuMYLg7wM_mtV0M5_9PCm764_0BkCkzs_zVAJTFKFhT-Aj0pD6Wne5XJuMPwhqwKqC3IxH0ljkMBTfHeApEXyEElPhdsJSk9l729gTEohprc1VimAs6qktsv3oPXx7zgH9Y0C2rxgEOs84Hyb9hPw=w409-h308-no</t>
+  </si>
+  <si>
+    <t>Grande traversée des Lofoten</t>
+  </si>
+  <si>
+    <t>Norvège</t>
+  </si>
+  <si>
+    <t>Juillet 2017</t>
+  </si>
+  <si>
+    <t>+1</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/ykMPu8fYsO9j8hTKM7wwwuTBvUCxsCjekf9DUqQAf8cQ565VQVmhRtrTqXmhlmikGPtmpxiWxJXHCepxip3cH92s8ubpRN8D4F4XiidluDZqMZXSzXk3OVwZ47olH-YBY56j_xLWImHvK_YpSTGlGTDg0lvS7qg9E8K8R2P7oB6dwpv4TSU045Y2iBy_T_FPIdbz-CHN3imKTpVAI23DwwEUGW7_nKM9lLYizPvFa9JbjeY7ao8zr2cKdzy0ilJAVQdfVHjH1kn6bg5t5ORfAKxc62aHrNlQkGtFbFrs1zL7i0Xmyo4WA_QWdezkStyb1HTexMSkmphD8Psrrr54u0L0rBXZ7dvjsobjO7M6Mu7h2kvmmCiZEooxjSJrJqx9o1qWO3ymEx5FHDCukta6KAJ7GoNnL32tc5F47BfVgFsUaeJRDW_7stvh-KuEQZosPllSULAjkPpAX_SM3Xznn4Sgu1lgrbzvQ2m0-DGyLe0H-_lIFselJlCs0Bf1M7EayTwrtuAenD23zeRJplDC8gOqZEwgK0T2xeOLjugiI1PlZ5bjGUz7afdNqufujS8fWhwZjq3ypG6261nd1_-WS0HveGM9_vDYPbTbJTb-lmT261Ui8udJ-VK7erNBspL0j_BZdcoyObsWPTVL9eJPKMaejMmMF4KS=w1680-h880-no</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -1178,7 +1189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1277,10 +1288,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1594,7 +1609,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2638,11 +2653,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X999"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145:XFD145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2654,14 +2669,14 @@
     <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -2684,14 +2699,22 @@
       <c r="W1" s="5"/>
       <c r="X1" s="5"/>
     </row>
-    <row r="2" spans="1:24">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
+    <row r="2" spans="1:25" s="19" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>341</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>342</v>
+      </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -2711,17 +2734,14 @@
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="Y2" s="5"/>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>16</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="4"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -2744,14 +2764,16 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:24" ht="120">
+    <row r="4" spans="1:25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="C4" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2774,12 +2796,12 @@
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
     </row>
-    <row r="5" spans="1:24" ht="90">
+    <row r="5" spans="1:25" ht="120">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>17</v>
+        <v>284</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="4"/>
@@ -2804,12 +2826,12 @@
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
     </row>
-    <row r="6" spans="1:24" ht="120">
+    <row r="6" spans="1:25" ht="90">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>286</v>
+        <v>17</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="4"/>
@@ -2834,12 +2856,12 @@
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
     </row>
-    <row r="7" spans="1:24" ht="60">
+    <row r="7" spans="1:25" ht="120">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>18</v>
+        <v>285</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="4"/>
@@ -2864,12 +2886,12 @@
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
     </row>
-    <row r="8" spans="1:24" ht="120">
+    <row r="8" spans="1:25" ht="60">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>287</v>
+        <v>18</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="4"/>
@@ -2894,12 +2916,12 @@
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
     </row>
-    <row r="9" spans="1:24" ht="75">
+    <row r="9" spans="1:25" ht="120">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>19</v>
+        <v>286</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="4"/>
@@ -2924,11 +2946,13 @@
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:25" ht="75">
       <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>19</v>
+      </c>
       <c r="C10" s="9"/>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
@@ -2952,9 +2976,9 @@
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:25">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -2980,19 +3004,13 @@
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:25">
       <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>22</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="4"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -3014,15 +3032,19 @@
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
     </row>
-    <row r="13" spans="1:24" ht="105">
+    <row r="13" spans="1:25">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -3044,12 +3066,12 @@
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
     </row>
-    <row r="14" spans="1:24" ht="120">
+    <row r="14" spans="1:25" ht="105">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>288</v>
+        <v>23</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="4"/>
@@ -3074,12 +3096,12 @@
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
     </row>
-    <row r="15" spans="1:24" ht="75">
+    <row r="15" spans="1:25" ht="120">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>24</v>
+        <v>287</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="4"/>
@@ -3104,12 +3126,12 @@
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
     </row>
-    <row r="16" spans="1:24" ht="135">
+    <row r="16" spans="1:25" ht="75">
       <c r="A16" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>289</v>
+        <v>24</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="4"/>
@@ -3134,12 +3156,12 @@
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
     </row>
-    <row r="17" spans="1:24" ht="45">
+    <row r="17" spans="1:24" ht="135">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>25</v>
+        <v>288</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="4"/>
@@ -3164,12 +3186,12 @@
       <c r="W17" s="5"/>
       <c r="X17" s="5"/>
     </row>
-    <row r="18" spans="1:24" ht="135">
+    <row r="18" spans="1:24" ht="45">
       <c r="A18" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>290</v>
+        <v>25</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="4"/>
@@ -3194,11 +3216,13 @@
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" ht="135">
       <c r="A19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>289</v>
+      </c>
       <c r="C19" s="9"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
@@ -3224,7 +3248,7 @@
     </row>
     <row r="20" spans="1:24">
       <c r="A20" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -3250,19 +3274,13 @@
       <c r="W20" s="5"/>
       <c r="X20" s="5"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1">
+    <row r="21" spans="1:24">
       <c r="A21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>28</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="4"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -3286,13 +3304,17 @@
     </row>
     <row r="22" spans="1:24" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -3316,14 +3338,12 @@
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>292</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C23" s="9"/>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -3348,12 +3368,14 @@
     </row>
     <row r="24" spans="1:24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="9"/>
+        <v>290</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>291</v>
+      </c>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -3378,10 +3400,10 @@
     </row>
     <row r="25" spans="1:24" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>293</v>
+        <v>30</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="4"/>
@@ -3408,10 +3430,10 @@
     </row>
     <row r="26" spans="1:24" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>31</v>
+        <v>292</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="4"/>
@@ -3438,10 +3460,10 @@
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>294</v>
+        <v>31</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="4"/>
@@ -3468,10 +3490,10 @@
     </row>
     <row r="28" spans="1:24" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>32</v>
+        <v>293</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="4"/>
@@ -3498,10 +3520,10 @@
     </row>
     <row r="29" spans="1:24" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>295</v>
+        <v>4</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="4"/>
@@ -3528,10 +3550,10 @@
     </row>
     <row r="30" spans="1:24" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>33</v>
+        <v>3</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>294</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="4"/>
@@ -3558,10 +3580,10 @@
     </row>
     <row r="31" spans="1:24" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>296</v>
+        <v>33</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="4"/>
@@ -3586,12 +3608,12 @@
       <c r="W31" s="5"/>
       <c r="X31" s="5"/>
     </row>
-    <row r="32" spans="1:24" ht="75">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>34</v>
+        <v>295</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="4"/>
@@ -3616,11 +3638,13 @@
       <c r="W32" s="5"/>
       <c r="X32" s="5"/>
     </row>
-    <row r="33" spans="1:24" ht="15.75" customHeight="1">
+    <row r="33" spans="1:24" ht="75">
       <c r="A33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="C33" s="9"/>
       <c r="D33" s="4"/>
       <c r="E33" s="5"/>
@@ -3646,7 +3670,7 @@
     </row>
     <row r="34" spans="1:24" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -3674,17 +3698,11 @@
     </row>
     <row r="35" spans="1:24" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>37</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="4"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -3708,13 +3726,17 @@
     </row>
     <row r="36" spans="1:24" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -3738,10 +3760,10 @@
     </row>
     <row r="37" spans="1:24" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>38</v>
+        <v>296</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="4"/>
@@ -3768,14 +3790,12 @@
     </row>
     <row r="38" spans="1:24" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>299</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C38" s="9"/>
       <c r="D38" s="4"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -3800,12 +3820,14 @@
     </row>
     <row r="39" spans="1:24" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="9"/>
+        <v>297</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>298</v>
+      </c>
       <c r="D39" s="4"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -3830,10 +3852,10 @@
     </row>
     <row r="40" spans="1:24" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>300</v>
+        <v>39</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="4"/>
@@ -3860,10 +3882,10 @@
     </row>
     <row r="41" spans="1:24" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>40</v>
+        <v>299</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="4"/>
@@ -3890,10 +3912,10 @@
     </row>
     <row r="42" spans="1:24" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>301</v>
+        <v>40</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="4"/>
@@ -3920,10 +3942,10 @@
     </row>
     <row r="43" spans="1:24" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>41</v>
+        <v>300</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="4"/>
@@ -3950,9 +3972,11 @@
     </row>
     <row r="44" spans="1:24" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B44" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="C44" s="9"/>
       <c r="D44" s="4"/>
       <c r="E44" s="5"/>
@@ -3978,7 +4002,7 @@
     </row>
     <row r="45" spans="1:24" ht="15.75" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -4006,17 +4030,11 @@
     </row>
     <row r="46" spans="1:24" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>44</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="4"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -4040,13 +4058,17 @@
     </row>
     <row r="47" spans="1:24" ht="15.75" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
@@ -4070,14 +4092,12 @@
     </row>
     <row r="48" spans="1:24" ht="15.75" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>303</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C48" s="9"/>
       <c r="D48" s="4"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -4102,12 +4122,14 @@
     </row>
     <row r="49" spans="1:24" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C49" s="9"/>
+        <v>301</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>302</v>
+      </c>
       <c r="D49" s="4"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -4132,10 +4154,10 @@
     </row>
     <row r="50" spans="1:24" ht="15.75" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>304</v>
+        <v>4</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="C50" s="9"/>
       <c r="D50" s="4"/>
@@ -4162,10 +4184,10 @@
     </row>
     <row r="51" spans="1:24" ht="15.75" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>47</v>
+        <v>3</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>303</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="4"/>
@@ -4192,10 +4214,10 @@
     </row>
     <row r="52" spans="1:24" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>305</v>
+        <v>4</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="4"/>
@@ -4222,10 +4244,10 @@
     </row>
     <row r="53" spans="1:24" ht="15.75" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>48</v>
+        <v>3</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>304</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="4"/>
@@ -4252,10 +4274,10 @@
     </row>
     <row r="54" spans="1:24" ht="15.75" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>306</v>
+        <v>4</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="4"/>
@@ -4282,10 +4304,10 @@
     </row>
     <row r="55" spans="1:24" ht="15.75" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>49</v>
+        <v>3</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="C55" s="9"/>
       <c r="D55" s="4"/>
@@ -4312,10 +4334,10 @@
     </row>
     <row r="56" spans="1:24" ht="15.75" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>307</v>
+        <v>4</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="4"/>
@@ -4342,10 +4364,10 @@
     </row>
     <row r="57" spans="1:24" ht="15.75" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>50</v>
+        <v>3</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>306</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="4"/>
@@ -4372,9 +4394,11 @@
     </row>
     <row r="58" spans="1:24" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B58" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>50</v>
+      </c>
       <c r="C58" s="9"/>
       <c r="D58" s="4"/>
       <c r="E58" s="5"/>
@@ -4400,7 +4424,7 @@
     </row>
     <row r="59" spans="1:24" ht="15.75" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -4428,17 +4452,11 @@
     </row>
     <row r="60" spans="1:24" ht="15.75" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D60" s="15" t="s">
-        <v>53</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="4"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
@@ -4462,13 +4480,17 @@
     </row>
     <row r="61" spans="1:24" ht="15.75" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="4"/>
+        <v>51</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>53</v>
+      </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
@@ -4492,14 +4514,12 @@
     </row>
     <row r="62" spans="1:24" ht="15.75" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>309</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C62" s="9"/>
       <c r="D62" s="4"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -4524,12 +4544,14 @@
     </row>
     <row r="63" spans="1:24" ht="15.75" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C63" s="9"/>
+        <v>307</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>308</v>
+      </c>
       <c r="D63" s="4"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
@@ -4554,10 +4576,10 @@
     </row>
     <row r="64" spans="1:24" ht="15.75" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>310</v>
+        <v>4</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="C64" s="9"/>
       <c r="D64" s="4"/>
@@ -4584,10 +4606,10 @@
     </row>
     <row r="65" spans="1:24" ht="15.75" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>56</v>
+        <v>3</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>309</v>
       </c>
       <c r="C65" s="9"/>
       <c r="D65" s="4"/>
@@ -4614,10 +4636,10 @@
     </row>
     <row r="66" spans="1:24" ht="15.75" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B66" s="15" t="s">
-        <v>311</v>
+        <v>4</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="C66" s="9"/>
       <c r="D66" s="4"/>
@@ -4644,10 +4666,10 @@
     </row>
     <row r="67" spans="1:24" ht="15.75" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B67" s="13" t="s">
-        <v>57</v>
+        <v>3</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>310</v>
       </c>
       <c r="C67" s="9"/>
       <c r="D67" s="4"/>
@@ -4674,9 +4696,11 @@
     </row>
     <row r="68" spans="1:24" ht="15.75" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B68" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>57</v>
+      </c>
       <c r="C68" s="9"/>
       <c r="D68" s="4"/>
       <c r="E68" s="5"/>
@@ -4702,7 +4726,7 @@
     </row>
     <row r="69" spans="1:24" ht="15.75" customHeight="1">
       <c r="A69" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -4730,17 +4754,11 @@
     </row>
     <row r="70" spans="1:24" ht="15.75" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D70" s="15" t="s">
-        <v>60</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B70" s="9"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="4"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
@@ -4764,13 +4782,17 @@
     </row>
     <row r="71" spans="1:24" ht="15.75" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C71" s="9"/>
-      <c r="D71" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
@@ -4794,10 +4816,10 @@
     </row>
     <row r="72" spans="1:24" ht="15.75" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B72" s="15" t="s">
-        <v>312</v>
+        <v>4</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="C72" s="9"/>
       <c r="D72" s="4"/>
@@ -4824,10 +4846,10 @@
     </row>
     <row r="73" spans="1:24" ht="15.75" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>62</v>
+        <v>3</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>311</v>
       </c>
       <c r="C73" s="9"/>
       <c r="D73" s="4"/>
@@ -4854,10 +4876,10 @@
     </row>
     <row r="74" spans="1:24" ht="15.75" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B74" s="15" t="s">
-        <v>313</v>
+        <v>4</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="C74" s="9"/>
       <c r="D74" s="4"/>
@@ -4884,10 +4906,10 @@
     </row>
     <row r="75" spans="1:24" ht="15.75" customHeight="1">
       <c r="A75" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B75" s="13" t="s">
-        <v>63</v>
+        <v>3</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>312</v>
       </c>
       <c r="C75" s="9"/>
       <c r="D75" s="4"/>
@@ -4914,10 +4936,10 @@
     </row>
     <row r="76" spans="1:24" ht="15.75" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B76" s="15" t="s">
-        <v>314</v>
+        <v>4</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="C76" s="9"/>
       <c r="D76" s="4"/>
@@ -4944,10 +4966,10 @@
     </row>
     <row r="77" spans="1:24" ht="15.75" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B77" s="13" t="s">
-        <v>64</v>
+        <v>3</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>313</v>
       </c>
       <c r="C77" s="9"/>
       <c r="D77" s="4"/>
@@ -4974,9 +4996,11 @@
     </row>
     <row r="78" spans="1:24" ht="15.75" customHeight="1">
       <c r="A78" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B78" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>64</v>
+      </c>
       <c r="C78" s="9"/>
       <c r="D78" s="4"/>
       <c r="E78" s="5"/>
@@ -5002,7 +5026,7 @@
     </row>
     <row r="79" spans="1:24" ht="15.75" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -5030,17 +5054,11 @@
     </row>
     <row r="80" spans="1:24" ht="15.75" customHeight="1">
       <c r="A80" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C80" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D80" s="15" t="s">
-        <v>67</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="4"/>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
       <c r="G80" s="5"/>
@@ -5064,13 +5082,17 @@
     </row>
     <row r="81" spans="1:24" ht="15.75" customHeight="1">
       <c r="A81" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C81" s="9"/>
-      <c r="D81" s="4"/>
+        <v>65</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>67</v>
+      </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
@@ -5094,10 +5116,10 @@
     </row>
     <row r="82" spans="1:24" ht="15.75" customHeight="1">
       <c r="A82" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>315</v>
+        <v>4</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="C82" s="9"/>
       <c r="D82" s="4"/>
@@ -5124,10 +5146,10 @@
     </row>
     <row r="83" spans="1:24" ht="15.75" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B83" s="13" t="s">
-        <v>69</v>
+        <v>3</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>314</v>
       </c>
       <c r="C83" s="9"/>
       <c r="D83" s="4"/>
@@ -5154,10 +5176,10 @@
     </row>
     <row r="84" spans="1:24" ht="15.75" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84" s="15" t="s">
-        <v>316</v>
+        <v>4</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="C84" s="9"/>
       <c r="D84" s="4"/>
@@ -5184,10 +5206,10 @@
     </row>
     <row r="85" spans="1:24" ht="15.75" customHeight="1">
       <c r="A85" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B85" s="13" t="s">
-        <v>70</v>
+        <v>3</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>315</v>
       </c>
       <c r="C85" s="9"/>
       <c r="D85" s="4"/>
@@ -5214,10 +5236,10 @@
     </row>
     <row r="86" spans="1:24" ht="15.75" customHeight="1">
       <c r="A86" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B86" s="15" t="s">
-        <v>317</v>
+        <v>4</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="C86" s="9"/>
       <c r="D86" s="4"/>
@@ -5244,10 +5266,10 @@
     </row>
     <row r="87" spans="1:24" ht="15.75" customHeight="1">
       <c r="A87" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B87" s="13" t="s">
-        <v>71</v>
+        <v>3</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>316</v>
       </c>
       <c r="C87" s="9"/>
       <c r="D87" s="4"/>
@@ -5274,9 +5296,11 @@
     </row>
     <row r="88" spans="1:24" ht="15.75" customHeight="1">
       <c r="A88" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B88" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>71</v>
+      </c>
       <c r="C88" s="9"/>
       <c r="D88" s="4"/>
       <c r="E88" s="5"/>
@@ -5302,7 +5326,7 @@
     </row>
     <row r="89" spans="1:24" ht="15.75" customHeight="1">
       <c r="A89" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -5330,17 +5354,11 @@
     </row>
     <row r="90" spans="1:24" ht="15.75" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B90" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C90" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D90" s="15" t="s">
-        <v>74</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B90" s="9"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="4"/>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
@@ -5364,13 +5382,17 @@
     </row>
     <row r="91" spans="1:24" ht="15.75" customHeight="1">
       <c r="A91" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C91" s="9"/>
-      <c r="D91" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>74</v>
+      </c>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -5394,10 +5416,10 @@
     </row>
     <row r="92" spans="1:24" ht="15.75" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B92" s="15" t="s">
-        <v>318</v>
+        <v>4</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="C92" s="9"/>
       <c r="D92" s="4"/>
@@ -5424,10 +5446,10 @@
     </row>
     <row r="93" spans="1:24" ht="15.75" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B93" s="13" t="s">
-        <v>76</v>
+        <v>3</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>317</v>
       </c>
       <c r="C93" s="9"/>
       <c r="D93" s="4"/>
@@ -5454,10 +5476,10 @@
     </row>
     <row r="94" spans="1:24" ht="15.75" customHeight="1">
       <c r="A94" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B94" s="15" t="s">
-        <v>319</v>
+        <v>4</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="C94" s="9"/>
       <c r="D94" s="4"/>
@@ -5484,10 +5506,10 @@
     </row>
     <row r="95" spans="1:24" ht="15.75" customHeight="1">
       <c r="A95" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B95" s="13" t="s">
-        <v>77</v>
+        <v>3</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>318</v>
       </c>
       <c r="C95" s="9"/>
       <c r="D95" s="4"/>
@@ -5514,14 +5536,12 @@
     </row>
     <row r="96" spans="1:24" ht="15.75" customHeight="1">
       <c r="A96" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B96" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="C96" s="10" t="s">
-        <v>321</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C96" s="9"/>
       <c r="D96" s="4"/>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
@@ -5544,14 +5564,16 @@
       <c r="W96" s="5"/>
       <c r="X96" s="5"/>
     </row>
-    <row r="97" spans="1:24" ht="75">
+    <row r="97" spans="1:24" ht="15.75" customHeight="1">
       <c r="A97" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B97" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C97" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>320</v>
+      </c>
       <c r="D97" s="4"/>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
@@ -5574,12 +5596,12 @@
       <c r="W97" s="5"/>
       <c r="X97" s="5"/>
     </row>
-    <row r="98" spans="1:24" ht="15.75" customHeight="1">
+    <row r="98" spans="1:24" ht="75">
       <c r="A98" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>323</v>
+        <v>78</v>
       </c>
       <c r="C98" s="9"/>
       <c r="D98" s="4"/>
@@ -5606,9 +5628,11 @@
     </row>
     <row r="99" spans="1:24" ht="15.75" customHeight="1">
       <c r="A99" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B99" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="B99" s="13" t="s">
+        <v>322</v>
+      </c>
       <c r="C99" s="9"/>
       <c r="D99" s="4"/>
       <c r="E99" s="5"/>
@@ -5634,7 +5658,7 @@
     </row>
     <row r="100" spans="1:24" ht="15.75" customHeight="1">
       <c r="A100" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
@@ -5662,17 +5686,11 @@
     </row>
     <row r="101" spans="1:24" ht="15.75" customHeight="1">
       <c r="A101" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B101" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C101" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D101" s="15" t="s">
-        <v>81</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B101" s="9"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="4"/>
       <c r="E101" s="5"/>
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
@@ -5696,13 +5714,17 @@
     </row>
     <row r="102" spans="1:24" ht="15.75" customHeight="1">
       <c r="A102" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C102" s="9"/>
-      <c r="D102" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D102" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
@@ -5726,10 +5748,10 @@
     </row>
     <row r="103" spans="1:24" ht="15.75" customHeight="1">
       <c r="A103" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>322</v>
+        <v>82</v>
       </c>
       <c r="C103" s="9"/>
       <c r="D103" s="4"/>
@@ -5754,12 +5776,12 @@
       <c r="W103" s="5"/>
       <c r="X103" s="5"/>
     </row>
-    <row r="104" spans="1:24" ht="45">
+    <row r="104" spans="1:24" ht="15.75" customHeight="1">
       <c r="A104" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>83</v>
+        <v>321</v>
       </c>
       <c r="C104" s="9"/>
       <c r="D104" s="4"/>
@@ -5784,13 +5806,14 @@
       <c r="W104" s="5"/>
       <c r="X104" s="5"/>
     </row>
-    <row r="105" spans="1:24" ht="15.75" customHeight="1">
+    <row r="105" spans="1:24" ht="45">
       <c r="A105" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B105" s="10" t="s">
-        <v>325</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C105" s="9"/>
       <c r="D105" s="4"/>
       <c r="E105" s="5"/>
       <c r="F105" s="5"/>
@@ -5815,12 +5838,11 @@
     </row>
     <row r="106" spans="1:24" ht="15.75" customHeight="1">
       <c r="A106" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B106" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C106" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>324</v>
+      </c>
       <c r="D106" s="4"/>
       <c r="E106" s="5"/>
       <c r="F106" s="5"/>
@@ -5845,10 +5867,10 @@
     </row>
     <row r="107" spans="1:24" ht="15.75" customHeight="1">
       <c r="A107" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>324</v>
+        <v>84</v>
       </c>
       <c r="C107" s="9"/>
       <c r="D107" s="4"/>
@@ -5875,10 +5897,10 @@
     </row>
     <row r="108" spans="1:24" ht="15.75" customHeight="1">
       <c r="A108" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>85</v>
+        <v>323</v>
       </c>
       <c r="C108" s="9"/>
       <c r="D108" s="4"/>
@@ -5903,15 +5925,15 @@
       <c r="W108" s="5"/>
       <c r="X108" s="5"/>
     </row>
-    <row r="109" spans="1:24" s="19" customFormat="1" ht="15.75" customHeight="1">
+    <row r="109" spans="1:24" ht="15.75" customHeight="1">
       <c r="A109" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="C109" s="10"/>
-      <c r="D109" s="16"/>
+        <v>85</v>
+      </c>
+      <c r="C109" s="9"/>
+      <c r="D109" s="4"/>
       <c r="E109" s="5"/>
       <c r="F109" s="5"/>
       <c r="G109" s="5"/>
@@ -5933,13 +5955,15 @@
       <c r="W109" s="5"/>
       <c r="X109" s="5"/>
     </row>
-    <row r="110" spans="1:24" ht="15.75" customHeight="1">
+    <row r="110" spans="1:24" s="19" customFormat="1" ht="15.75" customHeight="1">
       <c r="A110" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B110" s="9"/>
-      <c r="C110" s="9"/>
-      <c r="D110" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="B110" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C110" s="10"/>
+      <c r="D110" s="16"/>
       <c r="E110" s="5"/>
       <c r="F110" s="5"/>
       <c r="G110" s="5"/>
@@ -5963,7 +5987,7 @@
     </row>
     <row r="111" spans="1:24" ht="15.75" customHeight="1">
       <c r="A111" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
@@ -5991,17 +6015,11 @@
     </row>
     <row r="112" spans="1:24" ht="15.75" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C112" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D112" s="15" t="s">
-        <v>88</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B112" s="9"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="4"/>
       <c r="E112" s="5"/>
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
@@ -6025,13 +6043,17 @@
     </row>
     <row r="113" spans="1:24" ht="15.75" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C113" s="9"/>
-      <c r="D113" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D113" s="15" t="s">
+        <v>88</v>
+      </c>
       <c r="E113" s="5"/>
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
@@ -6055,14 +6077,12 @@
     </row>
     <row r="114" spans="1:24" ht="15.75" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="C114" s="13" t="s">
-        <v>328</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C114" s="9"/>
       <c r="D114" s="4"/>
       <c r="E114" s="5"/>
       <c r="F114" s="5"/>
@@ -6087,12 +6107,14 @@
     </row>
     <row r="115" spans="1:24" ht="15.75" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C115" s="9"/>
+        <v>326</v>
+      </c>
+      <c r="C115" s="13" t="s">
+        <v>327</v>
+      </c>
       <c r="D115" s="4"/>
       <c r="E115" s="5"/>
       <c r="F115" s="5"/>
@@ -6117,10 +6139,10 @@
     </row>
     <row r="116" spans="1:24" ht="15.75" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>329</v>
+        <v>90</v>
       </c>
       <c r="C116" s="9"/>
       <c r="D116" s="4"/>
@@ -6147,10 +6169,10 @@
     </row>
     <row r="117" spans="1:24" ht="15.75" customHeight="1">
       <c r="A117" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>91</v>
+        <v>328</v>
       </c>
       <c r="C117" s="9"/>
       <c r="D117" s="4"/>
@@ -6177,9 +6199,11 @@
     </row>
     <row r="118" spans="1:24" ht="15.75" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B118" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B118" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C118" s="9"/>
       <c r="D118" s="4"/>
       <c r="E118" s="5"/>
@@ -6205,7 +6229,7 @@
     </row>
     <row r="119" spans="1:24" ht="15.75" customHeight="1">
       <c r="A119" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
@@ -6233,17 +6257,11 @@
     </row>
     <row r="120" spans="1:24" ht="15.75" customHeight="1">
       <c r="A120" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B120" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C120" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D120" s="15" t="s">
-        <v>94</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B120" s="9"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="4"/>
       <c r="E120" s="5"/>
       <c r="F120" s="5"/>
       <c r="G120" s="5"/>
@@ -6267,13 +6285,17 @@
     </row>
     <row r="121" spans="1:24" ht="15.75" customHeight="1">
       <c r="A121" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C121" s="9"/>
-      <c r="D121" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="C121" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D121" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="E121" s="5"/>
       <c r="F121" s="5"/>
       <c r="G121" s="5"/>
@@ -6297,10 +6319,10 @@
     </row>
     <row r="122" spans="1:24" ht="15.75" customHeight="1">
       <c r="A122" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>330</v>
+        <v>95</v>
       </c>
       <c r="C122" s="9"/>
       <c r="D122" s="4"/>
@@ -6327,10 +6349,10 @@
     </row>
     <row r="123" spans="1:24" ht="15.75" customHeight="1">
       <c r="A123" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>96</v>
+        <v>329</v>
       </c>
       <c r="C123" s="9"/>
       <c r="D123" s="4"/>
@@ -6357,10 +6379,10 @@
     </row>
     <row r="124" spans="1:24" ht="15.75" customHeight="1">
       <c r="A124" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>331</v>
+        <v>96</v>
       </c>
       <c r="C124" s="9"/>
       <c r="D124" s="4"/>
@@ -6387,10 +6409,10 @@
     </row>
     <row r="125" spans="1:24" ht="15.75" customHeight="1">
       <c r="A125" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>97</v>
+        <v>330</v>
       </c>
       <c r="C125" s="9"/>
       <c r="D125" s="4"/>
@@ -6417,10 +6439,10 @@
     </row>
     <row r="126" spans="1:24" ht="15.75" customHeight="1">
       <c r="A126" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>332</v>
+        <v>97</v>
       </c>
       <c r="C126" s="9"/>
       <c r="D126" s="4"/>
@@ -6447,10 +6469,10 @@
     </row>
     <row r="127" spans="1:24" ht="15.75" customHeight="1">
       <c r="A127" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>98</v>
+        <v>331</v>
       </c>
       <c r="C127" s="9"/>
       <c r="D127" s="4"/>
@@ -6477,9 +6499,11 @@
     </row>
     <row r="128" spans="1:24" ht="15.75" customHeight="1">
       <c r="A128" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B128" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B128" s="13" t="s">
+        <v>98</v>
+      </c>
       <c r="C128" s="9"/>
       <c r="D128" s="4"/>
       <c r="E128" s="5"/>
@@ -6505,7 +6529,7 @@
     </row>
     <row r="129" spans="1:24" ht="15.75" customHeight="1">
       <c r="A129" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
@@ -6533,17 +6557,11 @@
     </row>
     <row r="130" spans="1:24" ht="15.75" customHeight="1">
       <c r="A130" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B130" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C130" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="D130" s="15" t="s">
-        <v>101</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B130" s="9"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="4"/>
       <c r="E130" s="5"/>
       <c r="F130" s="5"/>
       <c r="G130" s="5"/>
@@ -6567,13 +6585,17 @@
     </row>
     <row r="131" spans="1:24" ht="15.75" customHeight="1">
       <c r="A131" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C131" s="9"/>
-      <c r="D131" s="4"/>
+        <v>99</v>
+      </c>
+      <c r="C131" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D131" s="15" t="s">
+        <v>101</v>
+      </c>
       <c r="E131" s="5"/>
       <c r="F131" s="5"/>
       <c r="G131" s="5"/>
@@ -6597,10 +6619,10 @@
     </row>
     <row r="132" spans="1:24" ht="15.75" customHeight="1">
       <c r="A132" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>333</v>
+        <v>102</v>
       </c>
       <c r="C132" s="9"/>
       <c r="D132" s="4"/>
@@ -6627,10 +6649,10 @@
     </row>
     <row r="133" spans="1:24" ht="15.75" customHeight="1">
       <c r="A133" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>103</v>
+        <v>332</v>
       </c>
       <c r="C133" s="9"/>
       <c r="D133" s="4"/>
@@ -6657,10 +6679,10 @@
     </row>
     <row r="134" spans="1:24" ht="15.75" customHeight="1">
       <c r="A134" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>334</v>
+        <v>103</v>
       </c>
       <c r="C134" s="9"/>
       <c r="D134" s="4"/>
@@ -6687,10 +6709,10 @@
     </row>
     <row r="135" spans="1:24" ht="15.75" customHeight="1">
       <c r="A135" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>104</v>
+        <v>333</v>
       </c>
       <c r="C135" s="9"/>
       <c r="D135" s="4"/>
@@ -6717,10 +6739,10 @@
     </row>
     <row r="136" spans="1:24" ht="15.75" customHeight="1">
       <c r="A136" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>335</v>
+        <v>104</v>
       </c>
       <c r="C136" s="9"/>
       <c r="D136" s="4"/>
@@ -6747,10 +6769,10 @@
     </row>
     <row r="137" spans="1:24" ht="15.75" customHeight="1">
       <c r="A137" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>105</v>
+        <v>334</v>
       </c>
       <c r="C137" s="9"/>
       <c r="D137" s="4"/>
@@ -6777,9 +6799,11 @@
     </row>
     <row r="138" spans="1:24" ht="15.75" customHeight="1">
       <c r="A138" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B138" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B138" s="13" t="s">
+        <v>105</v>
+      </c>
       <c r="C138" s="9"/>
       <c r="D138" s="4"/>
       <c r="E138" s="5"/>
@@ -6805,7 +6829,7 @@
     </row>
     <row r="139" spans="1:24" ht="15.75" customHeight="1">
       <c r="A139" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B139" s="9"/>
       <c r="C139" s="9"/>
@@ -6833,14 +6857,10 @@
     </row>
     <row r="140" spans="1:24" ht="15.75" customHeight="1">
       <c r="A140" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B140" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C140" s="13" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B140" s="9"/>
+      <c r="C140" s="9"/>
       <c r="D140" s="4"/>
       <c r="E140" s="5"/>
       <c r="F140" s="5"/>
@@ -6863,14 +6883,16 @@
       <c r="W140" s="5"/>
       <c r="X140" s="5"/>
     </row>
-    <row r="141" spans="1:24" ht="120">
+    <row r="141" spans="1:24" ht="15.75" customHeight="1">
       <c r="A141" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B141" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="C141" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="B141" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="C141" s="13" t="s">
+        <v>106</v>
+      </c>
       <c r="D141" s="4"/>
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
@@ -6893,12 +6915,12 @@
       <c r="W141" s="5"/>
       <c r="X141" s="5"/>
     </row>
-    <row r="142" spans="1:24" ht="15.75" customHeight="1">
+    <row r="142" spans="1:24" ht="120">
       <c r="A142" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>336</v>
+        <v>107</v>
       </c>
       <c r="C142" s="9"/>
       <c r="D142" s="4"/>
@@ -6925,10 +6947,10 @@
     </row>
     <row r="143" spans="1:24" ht="15.75" customHeight="1">
       <c r="A143" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>109</v>
+        <v>335</v>
       </c>
       <c r="C143" s="9"/>
       <c r="D143" s="4"/>
@@ -6958,7 +6980,7 @@
         <v>4</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C144" s="9"/>
       <c r="D144" s="4"/>
@@ -6988,7 +7010,7 @@
         <v>4</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C145" s="9"/>
       <c r="D145" s="4"/>
@@ -7015,14 +7037,12 @@
     </row>
     <row r="146" spans="1:24" ht="15.75" customHeight="1">
       <c r="A146" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>337</v>
-      </c>
-      <c r="C146" s="10" t="s">
-        <v>338</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C146" s="9"/>
       <c r="D146" s="4"/>
       <c r="E146" s="5"/>
       <c r="F146" s="5"/>
@@ -7047,12 +7067,14 @@
     </row>
     <row r="147" spans="1:24" ht="15.75" customHeight="1">
       <c r="A147" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C147" s="9"/>
+        <v>336</v>
+      </c>
+      <c r="C147" s="10" t="s">
+        <v>337</v>
+      </c>
       <c r="D147" s="4"/>
       <c r="E147" s="5"/>
       <c r="F147" s="5"/>
@@ -7077,10 +7099,10 @@
     </row>
     <row r="148" spans="1:24" ht="15.75" customHeight="1">
       <c r="A148" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>339</v>
+        <v>111</v>
       </c>
       <c r="C148" s="9"/>
       <c r="D148" s="4"/>
@@ -7107,10 +7129,10 @@
     </row>
     <row r="149" spans="1:24" ht="15.75" customHeight="1">
       <c r="A149" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>113</v>
+        <v>338</v>
       </c>
       <c r="C149" s="9"/>
       <c r="D149" s="4"/>
@@ -7137,10 +7159,10 @@
     </row>
     <row r="150" spans="1:24" ht="15.75" customHeight="1">
       <c r="A150" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>340</v>
+        <v>112</v>
       </c>
       <c r="C150" s="9"/>
       <c r="D150" s="4"/>
@@ -7167,9 +7189,11 @@
     </row>
     <row r="151" spans="1:24" ht="15.75" customHeight="1">
       <c r="A151" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B151" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="B151" s="13" t="s">
+        <v>339</v>
+      </c>
       <c r="C151" s="9"/>
       <c r="D151" s="4"/>
       <c r="E151" s="5"/>
@@ -7193,7 +7217,34 @@
       <c r="W151" s="5"/>
       <c r="X151" s="5"/>
     </row>
-    <row r="152" spans="1:24" ht="15.75" customHeight="1"/>
+    <row r="152" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A152" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B152" s="9"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="5"/>
+      <c r="F152" s="5"/>
+      <c r="G152" s="5"/>
+      <c r="H152" s="5"/>
+      <c r="I152" s="5"/>
+      <c r="J152" s="5"/>
+      <c r="K152" s="5"/>
+      <c r="L152" s="5"/>
+      <c r="M152" s="5"/>
+      <c r="N152" s="5"/>
+      <c r="O152" s="5"/>
+      <c r="P152" s="5"/>
+      <c r="Q152" s="5"/>
+      <c r="R152" s="5"/>
+      <c r="S152" s="5"/>
+      <c r="T152" s="5"/>
+      <c r="U152" s="5"/>
+      <c r="V152" s="5"/>
+      <c r="W152" s="5"/>
+      <c r="X152" s="5"/>
+    </row>
     <row r="153" spans="1:24" ht="15.75" customHeight="1"/>
     <row r="154" spans="1:24" ht="15.75" customHeight="1"/>
     <row r="155" spans="1:24" ht="15.75" customHeight="1"/>
@@ -8041,6 +8092,7 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -8050,11 +8102,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>readme!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A151</xm:sqref>
+          <xm:sqref>A3:A152</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8063,11 +8115,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8084,10 +8136,10 @@
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -8113,19 +8165,19 @@
     </row>
     <row r="2" spans="1:25" ht="409.5">
       <c r="A2" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>232</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>233</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -8182,7 +8234,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="4"/>
@@ -8213,7 +8265,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="4"/>
@@ -8302,7 +8354,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="4"/>
@@ -8336,7 +8388,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
@@ -8366,7 +8418,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="4"/>
@@ -8397,7 +8449,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="4"/>
@@ -8428,7 +8480,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="4"/>
@@ -8459,13 +8511,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -8494,7 +8546,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="4"/>
@@ -8525,7 +8577,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="4"/>
@@ -8556,7 +8608,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="4"/>
@@ -8587,7 +8639,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="4"/>
@@ -8618,7 +8670,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="4"/>
@@ -8652,13 +8704,13 @@
         <v>29.3</v>
       </c>
       <c r="C19" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -8686,7 +8738,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="4"/>
@@ -8778,7 +8830,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
@@ -8808,7 +8860,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="4"/>
@@ -8839,13 +8891,13 @@
         <v>3</v>
       </c>
       <c r="B25" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>239</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>240</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -8874,7 +8926,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="4"/>
@@ -8905,7 +8957,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="4"/>
@@ -8936,7 +8988,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="4"/>
@@ -8967,7 +9019,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="4"/>
@@ -8998,7 +9050,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="15"/>
@@ -9029,7 +9081,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="4"/>
@@ -9060,7 +9112,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="4"/>
@@ -9091,7 +9143,7 @@
         <v>3</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="4"/>
@@ -9122,7 +9174,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="4"/>
@@ -9153,7 +9205,7 @@
         <v>3</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="4"/>
@@ -9184,7 +9236,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="4"/>
@@ -9218,13 +9270,13 @@
         <v>23.8</v>
       </c>
       <c r="C37" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="E37" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>152</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -9252,7 +9304,7 @@
         <v>6</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="4"/>
@@ -9344,7 +9396,7 @@
         <v>26</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="5"/>
@@ -9374,7 +9426,7 @@
         <v>4</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="4"/>
@@ -9405,7 +9457,7 @@
         <v>3</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="4"/>
@@ -9436,7 +9488,7 @@
         <v>4</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C44" s="13"/>
       <c r="D44" s="15"/>
@@ -9467,7 +9519,7 @@
         <v>3</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="4"/>
@@ -9498,7 +9550,7 @@
         <v>4</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="4"/>
@@ -9529,7 +9581,7 @@
         <v>4</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="4"/>
@@ -9563,13 +9615,13 @@
         <v>14.4</v>
       </c>
       <c r="C48" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="E48" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -9597,7 +9649,7 @@
         <v>6</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="4"/>
@@ -9689,7 +9741,7 @@
         <v>35</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="5"/>
@@ -9719,7 +9771,7 @@
         <v>4</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="4"/>
@@ -9750,7 +9802,7 @@
         <v>3</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="4"/>
@@ -9781,7 +9833,7 @@
         <v>4</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C55" s="9"/>
       <c r="D55" s="4"/>
@@ -9812,7 +9864,7 @@
         <v>3</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="4"/>
@@ -9843,7 +9895,7 @@
         <v>4</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="4"/>
@@ -9874,7 +9926,7 @@
         <v>3</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C58" s="13"/>
       <c r="D58" s="15"/>
@@ -9905,7 +9957,7 @@
         <v>4</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C59" s="9"/>
       <c r="D59" s="4"/>
@@ -9936,7 +9988,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C60" s="13"/>
       <c r="D60" s="4"/>
@@ -9967,7 +10019,7 @@
         <v>4</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C61" s="9"/>
       <c r="D61" s="4"/>
@@ -9998,7 +10050,7 @@
         <v>3</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C62" s="9"/>
       <c r="D62" s="4"/>
@@ -10029,7 +10081,7 @@
         <v>4</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C63" s="9"/>
       <c r="D63" s="4"/>
@@ -10063,13 +10115,13 @@
         <v>17.5</v>
       </c>
       <c r="C64" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="E64" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
@@ -10097,7 +10149,7 @@
         <v>6</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C65" s="9"/>
       <c r="D65" s="4"/>
@@ -10189,7 +10241,7 @@
         <v>42</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="5"/>
@@ -10219,7 +10271,7 @@
         <v>4</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C69" s="9"/>
       <c r="D69" s="4"/>
@@ -10250,7 +10302,7 @@
         <v>3</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="4"/>
@@ -10281,7 +10333,7 @@
         <v>4</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C71" s="9"/>
       <c r="D71" s="4"/>
@@ -10312,7 +10364,7 @@
         <v>3</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C72" s="9"/>
       <c r="D72" s="4"/>
@@ -10343,7 +10395,7 @@
         <v>4</v>
       </c>
       <c r="B73" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C73" s="9"/>
       <c r="D73" s="4"/>
@@ -10374,7 +10426,7 @@
         <v>3</v>
       </c>
       <c r="B74" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C74" s="9"/>
       <c r="D74" s="4"/>
@@ -10405,7 +10457,7 @@
         <v>4</v>
       </c>
       <c r="B75" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C75" s="9"/>
       <c r="D75" s="4"/>
@@ -10436,7 +10488,7 @@
         <v>3</v>
       </c>
       <c r="B76" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C76" s="9"/>
       <c r="D76" s="4"/>
@@ -10467,7 +10519,7 @@
         <v>4</v>
       </c>
       <c r="B77" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="15"/>
@@ -10498,7 +10550,7 @@
         <v>3</v>
       </c>
       <c r="B78" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="15"/>
@@ -10532,13 +10584,13 @@
         <v>19.5</v>
       </c>
       <c r="C79" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E79" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="F79" s="5"/>
       <c r="G79" s="5"/>
@@ -10566,7 +10618,7 @@
         <v>6</v>
       </c>
       <c r="B80" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C80" s="9"/>
       <c r="D80" s="4"/>
@@ -10658,7 +10710,7 @@
         <v>51</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="5"/>
@@ -10688,7 +10740,7 @@
         <v>4</v>
       </c>
       <c r="B84" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C84" s="9"/>
       <c r="D84" s="4"/>
@@ -10719,7 +10771,7 @@
         <v>3</v>
       </c>
       <c r="B85" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C85" s="9"/>
       <c r="D85" s="4"/>
@@ -10750,7 +10802,7 @@
         <v>4</v>
       </c>
       <c r="B86" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C86" s="9"/>
       <c r="D86" s="4"/>
@@ -10781,10 +10833,10 @@
         <v>3</v>
       </c>
       <c r="B87" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C87" s="10" t="s">
         <v>261</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>262</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="5"/>
@@ -10814,7 +10866,7 @@
         <v>4</v>
       </c>
       <c r="B88" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C88" s="9"/>
       <c r="D88" s="4"/>
@@ -10845,7 +10897,7 @@
         <v>3</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="5"/>
@@ -10875,7 +10927,7 @@
         <v>3</v>
       </c>
       <c r="B90" s="33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D90" s="16"/>
       <c r="E90" s="5"/>
@@ -10905,7 +10957,7 @@
         <v>4</v>
       </c>
       <c r="B91" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C91" s="13"/>
       <c r="D91" s="15"/>
@@ -10936,7 +10988,7 @@
         <v>3</v>
       </c>
       <c r="B92" s="20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C92" s="9"/>
       <c r="D92" s="4"/>
@@ -10970,13 +11022,13 @@
         <v>22</v>
       </c>
       <c r="C93" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D93" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="D93" s="23" t="s">
+      <c r="E93" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="F93" s="24"/>
       <c r="G93" s="24"/>
@@ -11005,7 +11057,7 @@
         <v>6</v>
       </c>
       <c r="B94" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C94" s="9"/>
       <c r="D94" s="4"/>
@@ -11097,7 +11149,7 @@
         <v>58</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="5"/>
@@ -11127,7 +11179,7 @@
         <v>4</v>
       </c>
       <c r="B98" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C98" s="9"/>
       <c r="D98" s="4"/>
@@ -11158,7 +11210,7 @@
         <v>4</v>
       </c>
       <c r="B99" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C99" s="9"/>
       <c r="D99" s="4"/>
@@ -11189,10 +11241,10 @@
         <v>3</v>
       </c>
       <c r="B100" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="C100" s="10" t="s">
         <v>266</v>
-      </c>
-      <c r="C100" s="10" t="s">
-        <v>267</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="5"/>
@@ -11222,7 +11274,7 @@
         <v>4</v>
       </c>
       <c r="B101" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C101" s="9"/>
       <c r="D101" s="4"/>
@@ -11253,7 +11305,7 @@
         <v>3</v>
       </c>
       <c r="B102" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C102" s="13"/>
       <c r="D102" s="15"/>
@@ -11284,7 +11336,7 @@
         <v>4</v>
       </c>
       <c r="B103" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C103" s="9"/>
       <c r="D103" s="4"/>
@@ -11315,7 +11367,7 @@
         <v>4</v>
       </c>
       <c r="B104" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C104" s="13"/>
       <c r="D104" s="4"/>
@@ -11346,7 +11398,7 @@
         <v>3</v>
       </c>
       <c r="B105" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C105" s="9"/>
       <c r="D105" s="4"/>
@@ -11377,7 +11429,7 @@
         <v>4</v>
       </c>
       <c r="B106" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C106" s="9"/>
       <c r="D106" s="4"/>
@@ -11411,13 +11463,13 @@
         <v>17.7</v>
       </c>
       <c r="C107" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D107" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E107" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="D107" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="E107" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="F107" s="5"/>
       <c r="G107" s="5"/>
@@ -11445,7 +11497,7 @@
         <v>6</v>
       </c>
       <c r="B108" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C108" s="13"/>
       <c r="D108" s="15"/>
@@ -11534,10 +11586,10 @@
         <v>2</v>
       </c>
       <c r="B111" s="34" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="5"/>
@@ -11567,7 +11619,7 @@
         <v>4</v>
       </c>
       <c r="B112" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C112" s="9"/>
       <c r="D112" s="4"/>
@@ -11598,7 +11650,7 @@
         <v>3</v>
       </c>
       <c r="B113" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C113" s="9"/>
       <c r="D113" s="4"/>
@@ -11629,7 +11681,7 @@
         <v>4</v>
       </c>
       <c r="B114" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C114" s="9"/>
       <c r="D114" s="4"/>
@@ -11660,7 +11712,7 @@
         <v>3</v>
       </c>
       <c r="B115" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C115" s="9"/>
       <c r="D115" s="4"/>
@@ -11691,7 +11743,7 @@
         <v>4</v>
       </c>
       <c r="B116" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C116" s="9"/>
       <c r="D116" s="4"/>
@@ -11722,7 +11774,7 @@
         <v>3</v>
       </c>
       <c r="B117" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C117" s="9"/>
       <c r="D117" s="4"/>
@@ -11753,7 +11805,7 @@
         <v>4</v>
       </c>
       <c r="B118" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C118" s="9"/>
       <c r="D118" s="4"/>
@@ -11784,10 +11836,10 @@
         <v>3</v>
       </c>
       <c r="B119" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="C119" s="13" t="s">
         <v>273</v>
-      </c>
-      <c r="C119" s="13" t="s">
-        <v>274</v>
       </c>
       <c r="D119" s="15"/>
       <c r="E119" s="5"/>
@@ -11820,13 +11872,13 @@
         <v>21.3</v>
       </c>
       <c r="C120" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D120" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="E120" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="E120" s="5" t="s">
-        <v>202</v>
       </c>
       <c r="F120" s="5"/>
       <c r="G120" s="5"/>
@@ -11854,7 +11906,7 @@
         <v>6</v>
       </c>
       <c r="B121" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C121" s="9"/>
       <c r="D121" s="4"/>
@@ -15438,7 +15490,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>readme!$B$2:$B$15</xm:f>
           </x14:formula1>
@@ -15451,11 +15503,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -15472,10 +15524,10 @@
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -15501,19 +15553,19 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" t="s">
         <v>228</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>230</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -15693,7 +15745,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
@@ -15754,7 +15806,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="4"/>
@@ -15785,13 +15837,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="16" t="s">
         <v>205</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>206</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -15820,7 +15872,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="13"/>
@@ -15851,7 +15903,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="4"/>
@@ -15882,7 +15934,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="4"/>
@@ -15913,7 +15965,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="4"/>
@@ -15944,7 +15996,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="4"/>
@@ -15975,7 +16027,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="4"/>
@@ -16006,7 +16058,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="4"/>
@@ -16037,13 +16089,13 @@
         <v>3</v>
       </c>
       <c r="B19" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="D19" s="16" t="s">
         <v>211</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>212</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -16072,7 +16124,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="4"/>
@@ -16103,7 +16155,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="4"/>
@@ -16134,7 +16186,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="4"/>
@@ -16226,7 +16278,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
@@ -16256,7 +16308,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="4"/>
@@ -16287,10 +16339,10 @@
         <v>3</v>
       </c>
       <c r="B27" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>214</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>215</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
@@ -16320,7 +16372,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
@@ -16351,7 +16403,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="4"/>
@@ -16382,13 +16434,13 @@
         <v>3</v>
       </c>
       <c r="B30" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="D30" s="16" t="s">
         <v>218</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>219</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -16417,7 +16469,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="4"/>
@@ -16448,7 +16500,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="4"/>
@@ -16479,7 +16531,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="15"/>
@@ -16510,7 +16562,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="4"/>
@@ -16541,7 +16593,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="4"/>
@@ -16630,7 +16682,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="4"/>
@@ -16661,7 +16713,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="4"/>
@@ -16692,7 +16744,7 @@
         <v>3</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="4"/>
@@ -16723,7 +16775,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="4"/>
@@ -16754,7 +16806,7 @@
         <v>3</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="4"/>
@@ -16785,7 +16837,7 @@
         <v>4</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="4"/>
@@ -16816,7 +16868,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="4"/>
@@ -22504,7 +22556,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>readme!$B$2:$B$15</xm:f>
           </x14:formula1>

</xml_diff>